<commit_message>
changes after presentation(s)...rewriting of text
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te_pres.xlsx
+++ b/Tables/decomposition_main_te_pres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ECFE30-890F-4863-A9D1-204DE0D9A4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E578C7-7D04-4CDC-97C1-36C552B74692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
+    <workbookView xWindow="6765" yWindow="1530" windowWidth="21600" windowHeight="11175" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition_main_te_pres1" sheetId="2" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -202,6 +199,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -728,7 +728,7 @@
   <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F12"/>
+      <selection activeCell="A2" sqref="A2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,13 +746,13 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="7"/>
       <c r="I2" s="6"/>
     </row>
@@ -760,16 +760,16 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -788,19 +788,19 @@
         <f>[1]decomposition_main_te!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C4" s="11" t="str">
+      <c r="C4" s="10" t="str">
         <f>[1]decomposition_main_te!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="11" t="str">
+      <c r="D4" s="10" t="str">
         <f>[1]decomposition_main_te!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E4" s="11" t="str">
+      <c r="E4" s="10" t="str">
         <f>[1]decomposition_main_te!E2</f>
         <v>(4)</v>
       </c>
-      <c r="F4" s="11" t="str">
+      <c r="F4" s="10" t="str">
         <f>[1]decomposition_main_te!F2</f>
         <v>(5)</v>
       </c>
@@ -822,19 +822,19 @@
         <f>[1]decomposition_main_te!B5</f>
         <v>-379.7***</v>
       </c>
-      <c r="C5" s="10" t="str">
+      <c r="C5" s="9" t="str">
         <f>[1]decomposition_main_te!C5</f>
         <v>-157.3***</v>
       </c>
-      <c r="D5" s="10" t="str">
+      <c r="D5" s="9" t="str">
         <f>[1]decomposition_main_te!D5</f>
         <v>32.1***</v>
       </c>
-      <c r="E5" s="10" t="str">
+      <c r="E5" s="9" t="str">
         <f>[1]decomposition_main_te!E5</f>
         <v>-0.57</v>
       </c>
-      <c r="F5" s="10" t="str">
+      <c r="F5" s="9" t="str">
         <f>[1]decomposition_main_te!F5</f>
         <v>-254.5**</v>
       </c>
@@ -856,19 +856,19 @@
         <f>[1]decomposition_main_te!B6</f>
         <v>(111.4)</v>
       </c>
-      <c r="C6" s="10" t="str">
+      <c r="C6" s="9" t="str">
         <f>[1]decomposition_main_te!C6</f>
         <v>(34.9)</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="9" t="str">
         <f>[1]decomposition_main_te!D6</f>
         <v>(1.43)</v>
       </c>
-      <c r="E6" s="10" t="str">
+      <c r="E6" s="9" t="str">
         <f>[1]decomposition_main_te!E6</f>
         <v>(3.03)</v>
       </c>
-      <c r="F6" s="10" t="str">
+      <c r="F6" s="9" t="str">
         <f>[1]decomposition_main_te!F6</f>
         <v>(104.8)</v>
       </c>
@@ -889,19 +889,19 @@
         <f>[1]decomposition_main_te!B8</f>
         <v>-84.9</v>
       </c>
-      <c r="C7" s="10" t="str">
+      <c r="C7" s="9" t="str">
         <f>[1]decomposition_main_te!C8</f>
         <v>-24.9</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="9" t="str">
         <f>[1]decomposition_main_te!D8</f>
         <v>1.34**</v>
       </c>
-      <c r="E7" s="10" t="str">
+      <c r="E7" s="9" t="str">
         <f>[1]decomposition_main_te!E8</f>
         <v>-3.98</v>
       </c>
-      <c r="F7" s="10" t="str">
+      <c r="F7" s="9" t="str">
         <f>[1]decomposition_main_te!F8</f>
         <v>-61.4</v>
       </c>
@@ -919,19 +919,19 @@
         <f>[1]decomposition_main_te!B9</f>
         <v>(114.6)</v>
       </c>
-      <c r="C8" s="10" t="str">
+      <c r="C8" s="9" t="str">
         <f>[1]decomposition_main_te!C9</f>
         <v>(38.4)</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="9" t="str">
         <f>[1]decomposition_main_te!D9</f>
         <v>(0.54)</v>
       </c>
-      <c r="E8" s="10" t="str">
+      <c r="E8" s="9" t="str">
         <f>[1]decomposition_main_te!E9</f>
         <v>(2.47)</v>
       </c>
-      <c r="F8" s="10" t="str">
+      <c r="F8" s="9" t="str">
         <f>[1]decomposition_main_te!F9</f>
         <v>(109.2)</v>
       </c>
@@ -945,10 +945,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -959,19 +959,19 @@
         <f>[1]decomposition_main_te!B11</f>
         <v>6304</v>
       </c>
-      <c r="C10" s="12" t="str">
+      <c r="C10" s="11" t="str">
         <f>[1]decomposition_main_te!C11</f>
         <v>6304</v>
       </c>
-      <c r="D10" s="12" t="str">
+      <c r="D10" s="11" t="str">
         <f>[1]decomposition_main_te!D11</f>
         <v>6304</v>
       </c>
-      <c r="E10" s="12" t="str">
+      <c r="E10" s="11" t="str">
         <f>[1]decomposition_main_te!E11</f>
         <v>6304</v>
       </c>
-      <c r="F10" s="12" t="str">
+      <c r="F10" s="11" t="str">
         <f>[1]decomposition_main_te!F11</f>
         <v>6304</v>
       </c>
@@ -993,19 +993,19 @@
         <f>[1]decomposition_main_te!B12</f>
         <v>0.007</v>
       </c>
-      <c r="C11" s="10" t="str">
+      <c r="C11" s="9" t="str">
         <f>[1]decomposition_main_te!C12</f>
         <v>0.022</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="9" t="str">
         <f>[1]decomposition_main_te!D12</f>
         <v>0.151</v>
       </c>
-      <c r="E11" s="10" t="str">
+      <c r="E11" s="9" t="str">
         <f>[1]decomposition_main_te!E12</f>
         <v>0.003</v>
       </c>
-      <c r="F11" s="10" t="str">
+      <c r="F11" s="9" t="str">
         <f>[1]decomposition_main_te!F12</f>
         <v>0.007</v>
       </c>
@@ -1026,19 +1026,19 @@
         <f>[1]decomposition_main_te!B13</f>
         <v>1851.0</v>
       </c>
-      <c r="C12" s="13" t="str">
+      <c r="C12" s="12" t="str">
         <f>[1]decomposition_main_te!C13</f>
         <v>545.9</v>
       </c>
-      <c r="D12" s="13" t="str">
+      <c r="D12" s="12" t="str">
         <f>[1]decomposition_main_te!D13</f>
         <v>0</v>
       </c>
-      <c r="E12" s="13" t="str">
+      <c r="E12" s="12" t="str">
         <f>[1]decomposition_main_te!E13</f>
         <v>5.82</v>
       </c>
-      <c r="F12" s="13" t="str">
+      <c r="F12" s="12" t="str">
         <f>[1]decomposition_main_te!F13</f>
         <v>1305.1</v>
       </c>
@@ -1085,13 +1085,13 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="7"/>
       <c r="I2" s="6"/>
     </row>

</xml_diff>